<commit_message>
bugs n custom loss
ska
</commit_message>
<xml_diff>
--- a/Solar Forecasting/Parameter Tuning.xlsx
+++ b/Solar Forecasting/Parameter Tuning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df56bcf1b7338548/Documents/GitHub/SeniorDesign/Solar Forecasting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{3B470B55-7330-44D8-A21D-CC8B057923D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6F468C4-1075-4CC8-A033-014D40789EC8}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{3B470B55-7330-44D8-A21D-CC8B057923D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4192C22D-F102-456A-A5CD-CDE2C798DC16}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{65110851-02A7-4AC7-90E9-6DC6385F35E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>Solar Forecasting Parameter Tuning :)</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Removed index layer</t>
+  </si>
+  <si>
+    <t>Test size reduced from 0.33 to 0.2</t>
   </si>
 </sst>
 </file>
@@ -611,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045A7848-BF7C-4FC5-A423-83BCCEC5BCDD}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1046,17 +1049,35 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="8"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="8">
+        <v>13</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="7">
+        <v>300</v>
+      </c>
+      <c r="J17" s="7">
+        <v>10</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>